<commit_message>
sampai bikin baris baru
</commit_message>
<xml_diff>
--- a/application/libraries/excel/template - Copy.xlsx
+++ b/application/libraries/excel/template - Copy.xlsx
@@ -18,6 +18,7 @@
     <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$1:$15</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -365,25 +366,85 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="15" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -391,69 +452,7 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -737,7 +736,7 @@
   <dimension ref="A1:AI18"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageLayout" zoomScale="70" zoomScaleNormal="55" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="K25" sqref="K25"/>
+      <selection activeCell="O19" sqref="O19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -758,43 +757,43 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:35" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="9"/>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-      <c r="H1" s="37" t="s">
+      <c r="A1" s="7"/>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="I1" s="37"/>
-      <c r="J1" s="37"/>
-      <c r="K1" s="37"/>
-      <c r="L1" s="37"/>
-      <c r="M1" s="37"/>
-      <c r="N1" s="37"/>
-      <c r="O1" s="37"/>
-      <c r="P1" s="37"/>
-      <c r="Q1" s="37"/>
-      <c r="R1" s="37"/>
-      <c r="S1" s="37"/>
-      <c r="T1" s="37"/>
-      <c r="U1" s="37"/>
-      <c r="V1" s="37"/>
-      <c r="W1" s="37"/>
-      <c r="X1" s="37"/>
-      <c r="Y1" s="37"/>
-      <c r="Z1" s="9"/>
-      <c r="AA1" s="9"/>
-      <c r="AB1" s="9"/>
-      <c r="AC1" s="9"/>
-      <c r="AD1" s="9"/>
-      <c r="AE1" s="9"/>
-      <c r="AF1" s="9"/>
-      <c r="AG1" s="9"/>
-      <c r="AH1" s="9"/>
-      <c r="AI1" s="9"/>
+      <c r="I1" s="9"/>
+      <c r="J1" s="9"/>
+      <c r="K1" s="9"/>
+      <c r="L1" s="9"/>
+      <c r="M1" s="9"/>
+      <c r="N1" s="9"/>
+      <c r="O1" s="9"/>
+      <c r="P1" s="9"/>
+      <c r="Q1" s="9"/>
+      <c r="R1" s="9"/>
+      <c r="S1" s="9"/>
+      <c r="T1" s="9"/>
+      <c r="U1" s="9"/>
+      <c r="V1" s="9"/>
+      <c r="W1" s="9"/>
+      <c r="X1" s="9"/>
+      <c r="Y1" s="9"/>
+      <c r="Z1" s="7"/>
+      <c r="AA1" s="7"/>
+      <c r="AB1" s="7"/>
+      <c r="AC1" s="7"/>
+      <c r="AD1" s="7"/>
+      <c r="AE1" s="7"/>
+      <c r="AF1" s="7"/>
+      <c r="AG1" s="7"/>
+      <c r="AH1" s="7"/>
+      <c r="AI1" s="7"/>
     </row>
     <row r="2" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
@@ -881,128 +880,128 @@
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
-      <c r="K4" s="13" t="s">
+      <c r="K4" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="L4" s="13"/>
-      <c r="M4" s="13"/>
-      <c r="N4" s="13"/>
-      <c r="O4" s="13" t="s">
+      <c r="L4" s="25"/>
+      <c r="M4" s="25"/>
+      <c r="N4" s="25"/>
+      <c r="O4" s="25" t="s">
         <v>36</v>
       </c>
-      <c r="P4" s="13"/>
-      <c r="Q4" s="13"/>
-      <c r="R4" s="13"/>
-      <c r="S4" s="13"/>
-      <c r="T4" s="13"/>
+      <c r="P4" s="25"/>
+      <c r="Q4" s="25"/>
+      <c r="R4" s="25"/>
+      <c r="S4" s="25"/>
+      <c r="T4" s="25"/>
       <c r="U4" s="1"/>
       <c r="V4" s="1"/>
       <c r="W4" s="1"/>
       <c r="X4" s="1"/>
       <c r="Y4" s="1"/>
-      <c r="Z4" s="13" t="s">
+      <c r="Z4" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="AA4" s="13"/>
-      <c r="AB4" s="13"/>
-      <c r="AC4" s="13" t="s">
+      <c r="AA4" s="25"/>
+      <c r="AB4" s="25"/>
+      <c r="AC4" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="AD4" s="13"/>
-      <c r="AE4" s="13"/>
-      <c r="AF4" s="13"/>
+      <c r="AD4" s="25"/>
+      <c r="AE4" s="25"/>
+      <c r="AF4" s="25"/>
       <c r="AG4" s="6"/>
       <c r="AH4" s="6"/>
       <c r="AI4" s="6"/>
     </row>
     <row r="5" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="14" t="s">
+      <c r="A5" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="14"/>
-      <c r="C5" s="14"/>
-      <c r="D5" s="14"/>
-      <c r="E5" s="14"/>
-      <c r="F5" s="14"/>
-      <c r="G5" s="14"/>
-      <c r="H5" s="14"/>
+      <c r="B5" s="34"/>
+      <c r="C5" s="34"/>
+      <c r="D5" s="34"/>
+      <c r="E5" s="34"/>
+      <c r="F5" s="34"/>
+      <c r="G5" s="34"/>
+      <c r="H5" s="34"/>
       <c r="I5" s="4"/>
       <c r="J5" s="2"/>
-      <c r="K5" s="13" t="s">
+      <c r="K5" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="L5" s="13"/>
-      <c r="M5" s="13"/>
-      <c r="N5" s="13"/>
-      <c r="O5" s="15" t="s">
+      <c r="L5" s="25"/>
+      <c r="M5" s="25"/>
+      <c r="N5" s="25"/>
+      <c r="O5" s="35" t="s">
         <v>37</v>
       </c>
-      <c r="P5" s="15"/>
-      <c r="Q5" s="15"/>
-      <c r="R5" s="15"/>
-      <c r="S5" s="15"/>
-      <c r="T5" s="15"/>
+      <c r="P5" s="35"/>
+      <c r="Q5" s="35"/>
+      <c r="R5" s="35"/>
+      <c r="S5" s="35"/>
+      <c r="T5" s="35"/>
       <c r="U5" s="1"/>
       <c r="V5" s="1"/>
       <c r="W5" s="1"/>
       <c r="X5" s="1"/>
       <c r="Y5" s="1"/>
-      <c r="Z5" s="16" t="s">
+      <c r="Z5" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="AA5" s="16"/>
-      <c r="AB5" s="16"/>
-      <c r="AC5" s="13" t="s">
+      <c r="AA5" s="36"/>
+      <c r="AB5" s="36"/>
+      <c r="AC5" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="AD5" s="13"/>
-      <c r="AE5" s="13"/>
-      <c r="AF5" s="13"/>
+      <c r="AD5" s="25"/>
+      <c r="AE5" s="25"/>
+      <c r="AF5" s="25"/>
       <c r="AG5" s="6"/>
       <c r="AH5" s="6"/>
       <c r="AI5" s="6"/>
     </row>
     <row r="6" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="14"/>
-      <c r="B6" s="14"/>
-      <c r="C6" s="14"/>
-      <c r="D6" s="14"/>
-      <c r="E6" s="14"/>
-      <c r="F6" s="14"/>
-      <c r="G6" s="14"/>
-      <c r="H6" s="14"/>
+      <c r="A6" s="34"/>
+      <c r="B6" s="34"/>
+      <c r="C6" s="34"/>
+      <c r="D6" s="34"/>
+      <c r="E6" s="34"/>
+      <c r="F6" s="34"/>
+      <c r="G6" s="34"/>
+      <c r="H6" s="34"/>
       <c r="I6" s="4"/>
       <c r="J6" s="2"/>
-      <c r="K6" s="13" t="s">
+      <c r="K6" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="L6" s="13"/>
-      <c r="M6" s="13"/>
-      <c r="N6" s="13"/>
-      <c r="O6" s="13" t="s">
+      <c r="L6" s="25"/>
+      <c r="M6" s="25"/>
+      <c r="N6" s="25"/>
+      <c r="O6" s="25" t="s">
         <v>38</v>
       </c>
-      <c r="P6" s="13"/>
-      <c r="Q6" s="13"/>
-      <c r="R6" s="13"/>
-      <c r="S6" s="13"/>
-      <c r="T6" s="13"/>
+      <c r="P6" s="25"/>
+      <c r="Q6" s="25"/>
+      <c r="R6" s="25"/>
+      <c r="S6" s="25"/>
+      <c r="T6" s="25"/>
       <c r="U6" s="1"/>
       <c r="V6" s="1"/>
       <c r="W6" s="1"/>
       <c r="X6" s="1"/>
       <c r="Y6" s="1"/>
-      <c r="Z6" s="13" t="s">
+      <c r="Z6" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="AA6" s="13"/>
-      <c r="AB6" s="13"/>
-      <c r="AC6" s="13" t="s">
+      <c r="AA6" s="25"/>
+      <c r="AB6" s="25"/>
+      <c r="AC6" s="25" t="s">
         <v>39</v>
       </c>
-      <c r="AD6" s="13"/>
-      <c r="AE6" s="13"/>
-      <c r="AF6" s="13"/>
+      <c r="AD6" s="25"/>
+      <c r="AE6" s="25"/>
+      <c r="AF6" s="25"/>
       <c r="AG6" s="6"/>
       <c r="AH6" s="6"/>
       <c r="AI6" s="5"/>
@@ -1018,25 +1017,25 @@
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
-      <c r="K7" s="26" t="s">
+      <c r="K7" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="L7" s="26"/>
-      <c r="M7" s="26"/>
-      <c r="N7" s="26"/>
-      <c r="O7" s="26" t="s">
+      <c r="L7" s="32"/>
+      <c r="M7" s="32"/>
+      <c r="N7" s="32"/>
+      <c r="O7" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="P7" s="26"/>
-      <c r="Q7" s="26"/>
-      <c r="R7" s="26"/>
-      <c r="S7" s="26"/>
-      <c r="T7" s="26"/>
-      <c r="U7" s="26"/>
-      <c r="V7" s="26"/>
-      <c r="W7" s="26"/>
-      <c r="X7" s="26"/>
-      <c r="Y7" s="26"/>
+      <c r="P7" s="32"/>
+      <c r="Q7" s="32"/>
+      <c r="R7" s="32"/>
+      <c r="S7" s="32"/>
+      <c r="T7" s="32"/>
+      <c r="U7" s="32"/>
+      <c r="V7" s="32"/>
+      <c r="W7" s="32"/>
+      <c r="X7" s="32"/>
+      <c r="Y7" s="32"/>
       <c r="Z7" s="1"/>
       <c r="AA7" s="1"/>
       <c r="AB7" s="1"/>
@@ -1049,440 +1048,440 @@
       <c r="AI7" s="5"/>
     </row>
     <row r="8" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="20" t="s">
+      <c r="A8" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="21"/>
-      <c r="C8" s="21"/>
-      <c r="D8" s="21"/>
-      <c r="E8" s="21"/>
-      <c r="F8" s="21"/>
-      <c r="G8" s="21"/>
-      <c r="H8" s="21"/>
-      <c r="I8" s="21"/>
-      <c r="J8" s="21"/>
-      <c r="K8" s="21"/>
-      <c r="L8" s="21"/>
-      <c r="M8" s="21"/>
-      <c r="N8" s="21"/>
-      <c r="O8" s="21"/>
-      <c r="P8" s="21"/>
-      <c r="Q8" s="21"/>
-      <c r="R8" s="21"/>
-      <c r="S8" s="21"/>
-      <c r="T8" s="21"/>
-      <c r="U8" s="21"/>
-      <c r="V8" s="21"/>
-      <c r="W8" s="21"/>
-      <c r="X8" s="21"/>
-      <c r="Y8" s="21"/>
-      <c r="Z8" s="21"/>
-      <c r="AA8" s="22"/>
-      <c r="AB8" s="29" t="s">
+      <c r="B8" s="27"/>
+      <c r="C8" s="27"/>
+      <c r="D8" s="27"/>
+      <c r="E8" s="27"/>
+      <c r="F8" s="27"/>
+      <c r="G8" s="27"/>
+      <c r="H8" s="27"/>
+      <c r="I8" s="27"/>
+      <c r="J8" s="27"/>
+      <c r="K8" s="27"/>
+      <c r="L8" s="27"/>
+      <c r="M8" s="27"/>
+      <c r="N8" s="27"/>
+      <c r="O8" s="27"/>
+      <c r="P8" s="27"/>
+      <c r="Q8" s="27"/>
+      <c r="R8" s="27"/>
+      <c r="S8" s="27"/>
+      <c r="T8" s="27"/>
+      <c r="U8" s="27"/>
+      <c r="V8" s="27"/>
+      <c r="W8" s="27"/>
+      <c r="X8" s="27"/>
+      <c r="Y8" s="27"/>
+      <c r="Z8" s="27"/>
+      <c r="AA8" s="28"/>
+      <c r="AB8" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="AC8" s="30"/>
-      <c r="AD8" s="27" t="s">
+      <c r="AC8" s="20"/>
+      <c r="AD8" s="33" t="s">
         <v>11</v>
       </c>
-      <c r="AE8" s="27"/>
-      <c r="AF8" s="27"/>
-      <c r="AG8" s="27"/>
-      <c r="AH8" s="27" t="s">
+      <c r="AE8" s="33"/>
+      <c r="AF8" s="33"/>
+      <c r="AG8" s="33"/>
+      <c r="AH8" s="33" t="s">
         <v>12</v>
       </c>
-      <c r="AI8" s="27"/>
+      <c r="AI8" s="33"/>
     </row>
     <row r="9" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="23"/>
-      <c r="B9" s="24"/>
-      <c r="C9" s="24"/>
-      <c r="D9" s="24"/>
-      <c r="E9" s="24"/>
-      <c r="F9" s="24"/>
-      <c r="G9" s="24"/>
-      <c r="H9" s="24"/>
-      <c r="I9" s="24"/>
-      <c r="J9" s="24"/>
-      <c r="K9" s="24"/>
-      <c r="L9" s="24"/>
-      <c r="M9" s="24"/>
-      <c r="N9" s="24"/>
-      <c r="O9" s="24"/>
-      <c r="P9" s="24"/>
-      <c r="Q9" s="24"/>
-      <c r="R9" s="24"/>
-      <c r="S9" s="24"/>
-      <c r="T9" s="24"/>
-      <c r="U9" s="24"/>
-      <c r="V9" s="24"/>
-      <c r="W9" s="24"/>
-      <c r="X9" s="24"/>
-      <c r="Y9" s="24"/>
-      <c r="Z9" s="24"/>
-      <c r="AA9" s="25"/>
-      <c r="AB9" s="31"/>
-      <c r="AC9" s="32"/>
-      <c r="AD9" s="27"/>
-      <c r="AE9" s="27"/>
-      <c r="AF9" s="27"/>
-      <c r="AG9" s="27"/>
-      <c r="AH9" s="27"/>
-      <c r="AI9" s="27"/>
+      <c r="A9" s="29"/>
+      <c r="B9" s="30"/>
+      <c r="C9" s="30"/>
+      <c r="D9" s="30"/>
+      <c r="E9" s="30"/>
+      <c r="F9" s="30"/>
+      <c r="G9" s="30"/>
+      <c r="H9" s="30"/>
+      <c r="I9" s="30"/>
+      <c r="J9" s="30"/>
+      <c r="K9" s="30"/>
+      <c r="L9" s="30"/>
+      <c r="M9" s="30"/>
+      <c r="N9" s="30"/>
+      <c r="O9" s="30"/>
+      <c r="P9" s="30"/>
+      <c r="Q9" s="30"/>
+      <c r="R9" s="30"/>
+      <c r="S9" s="30"/>
+      <c r="T9" s="30"/>
+      <c r="U9" s="30"/>
+      <c r="V9" s="30"/>
+      <c r="W9" s="30"/>
+      <c r="X9" s="30"/>
+      <c r="Y9" s="30"/>
+      <c r="Z9" s="30"/>
+      <c r="AA9" s="31"/>
+      <c r="AB9" s="21"/>
+      <c r="AC9" s="22"/>
+      <c r="AD9" s="33"/>
+      <c r="AE9" s="33"/>
+      <c r="AF9" s="33"/>
+      <c r="AG9" s="33"/>
+      <c r="AH9" s="33"/>
+      <c r="AI9" s="33"/>
     </row>
     <row r="10" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="19" t="s">
+      <c r="A10" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="19"/>
-      <c r="C10" s="19"/>
-      <c r="D10" s="17" t="s">
+      <c r="B10" s="11"/>
+      <c r="C10" s="11"/>
+      <c r="D10" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="E10" s="18"/>
-      <c r="F10" s="19" t="s">
+      <c r="E10" s="16"/>
+      <c r="F10" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="G10" s="19"/>
-      <c r="H10" s="19" t="s">
+      <c r="G10" s="11"/>
+      <c r="H10" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="I10" s="19"/>
-      <c r="J10" s="19" t="s">
+      <c r="I10" s="11"/>
+      <c r="J10" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="K10" s="19"/>
-      <c r="L10" s="19" t="s">
+      <c r="K10" s="11"/>
+      <c r="L10" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="M10" s="19"/>
-      <c r="N10" s="19" t="s">
+      <c r="M10" s="11"/>
+      <c r="N10" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="O10" s="28"/>
-      <c r="P10" s="19" t="s">
+      <c r="O10" s="18"/>
+      <c r="P10" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="Q10" s="19"/>
-      <c r="R10" s="19" t="s">
+      <c r="Q10" s="11"/>
+      <c r="R10" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="S10" s="19"/>
-      <c r="T10" s="19"/>
-      <c r="U10" s="19" t="s">
+      <c r="S10" s="11"/>
+      <c r="T10" s="11"/>
+      <c r="U10" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="V10" s="19"/>
-      <c r="W10" s="19"/>
-      <c r="X10" s="19" t="s">
+      <c r="V10" s="11"/>
+      <c r="W10" s="11"/>
+      <c r="X10" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="Y10" s="19"/>
-      <c r="Z10" s="17" t="s">
+      <c r="Y10" s="11"/>
+      <c r="Z10" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="AA10" s="18"/>
-      <c r="AB10" s="33"/>
-      <c r="AC10" s="34"/>
-      <c r="AD10" s="27"/>
-      <c r="AE10" s="27"/>
-      <c r="AF10" s="27"/>
-      <c r="AG10" s="27"/>
-      <c r="AH10" s="27"/>
-      <c r="AI10" s="27"/>
+      <c r="AA10" s="16"/>
+      <c r="AB10" s="23"/>
+      <c r="AC10" s="24"/>
+      <c r="AD10" s="33"/>
+      <c r="AE10" s="33"/>
+      <c r="AF10" s="33"/>
+      <c r="AG10" s="33"/>
+      <c r="AH10" s="33"/>
+      <c r="AI10" s="33"/>
     </row>
     <row r="11" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="19">
+      <c r="A11" s="11">
         <v>0</v>
       </c>
-      <c r="B11" s="19"/>
-      <c r="C11" s="19"/>
-      <c r="D11" s="19">
+      <c r="B11" s="11"/>
+      <c r="C11" s="11"/>
+      <c r="D11" s="11">
         <v>0</v>
       </c>
-      <c r="E11" s="19"/>
-      <c r="F11" s="19">
+      <c r="E11" s="11"/>
+      <c r="F11" s="11">
         <v>0</v>
       </c>
-      <c r="G11" s="19"/>
-      <c r="H11" s="19">
+      <c r="G11" s="11"/>
+      <c r="H11" s="11">
         <v>0</v>
       </c>
-      <c r="I11" s="19"/>
-      <c r="J11" s="19">
+      <c r="I11" s="11"/>
+      <c r="J11" s="11">
         <v>0</v>
       </c>
-      <c r="K11" s="19"/>
-      <c r="L11" s="19">
+      <c r="K11" s="11"/>
+      <c r="L11" s="11">
         <v>0</v>
       </c>
-      <c r="M11" s="19"/>
-      <c r="N11" s="19">
+      <c r="M11" s="11"/>
+      <c r="N11" s="11">
         <v>0</v>
       </c>
-      <c r="O11" s="19"/>
-      <c r="P11" s="19">
+      <c r="O11" s="11"/>
+      <c r="P11" s="11">
         <v>0</v>
       </c>
-      <c r="Q11" s="19"/>
-      <c r="R11" s="19">
+      <c r="Q11" s="11"/>
+      <c r="R11" s="11">
         <v>0</v>
       </c>
-      <c r="S11" s="19"/>
-      <c r="T11" s="19"/>
-      <c r="U11" s="19">
+      <c r="S11" s="11"/>
+      <c r="T11" s="11"/>
+      <c r="U11" s="11">
         <v>0</v>
       </c>
-      <c r="V11" s="19"/>
-      <c r="W11" s="19"/>
-      <c r="X11" s="19">
+      <c r="V11" s="11"/>
+      <c r="W11" s="11"/>
+      <c r="X11" s="11">
         <v>0</v>
       </c>
-      <c r="Y11" s="19"/>
-      <c r="Z11" s="17">
+      <c r="Y11" s="11"/>
+      <c r="Z11" s="14">
         <v>0</v>
       </c>
-      <c r="AA11" s="18"/>
-      <c r="AB11" s="17"/>
-      <c r="AC11" s="18"/>
-      <c r="AD11" s="19">
+      <c r="AA11" s="16"/>
+      <c r="AB11" s="14"/>
+      <c r="AC11" s="16"/>
+      <c r="AD11" s="11">
         <v>0</v>
       </c>
-      <c r="AE11" s="19"/>
-      <c r="AF11" s="19"/>
-      <c r="AG11" s="19"/>
-      <c r="AH11" s="19">
+      <c r="AE11" s="11"/>
+      <c r="AF11" s="11"/>
+      <c r="AG11" s="11"/>
+      <c r="AH11" s="11">
         <v>0</v>
       </c>
-      <c r="AI11" s="19"/>
+      <c r="AI11" s="11"/>
     </row>
     <row r="12" spans="1:35" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="17"/>
-      <c r="B12" s="36"/>
-      <c r="C12" s="36"/>
-      <c r="D12" s="36"/>
-      <c r="E12" s="36"/>
-      <c r="F12" s="36"/>
-      <c r="G12" s="36"/>
-      <c r="H12" s="36"/>
-      <c r="I12" s="36"/>
-      <c r="J12" s="36"/>
-      <c r="K12" s="36"/>
-      <c r="L12" s="36"/>
-      <c r="M12" s="36"/>
-      <c r="N12" s="36"/>
-      <c r="O12" s="36"/>
-      <c r="P12" s="36"/>
-      <c r="Q12" s="36"/>
-      <c r="R12" s="36"/>
-      <c r="S12" s="36"/>
-      <c r="T12" s="36"/>
-      <c r="U12" s="36"/>
-      <c r="V12" s="36"/>
-      <c r="W12" s="36"/>
-      <c r="X12" s="36"/>
-      <c r="Y12" s="36"/>
-      <c r="Z12" s="36"/>
-      <c r="AA12" s="36"/>
-      <c r="AB12" s="36"/>
-      <c r="AC12" s="36"/>
-      <c r="AD12" s="36"/>
-      <c r="AE12" s="36"/>
-      <c r="AF12" s="36"/>
-      <c r="AG12" s="36"/>
-      <c r="AH12" s="36"/>
-      <c r="AI12" s="18"/>
+      <c r="A12" s="14"/>
+      <c r="B12" s="15"/>
+      <c r="C12" s="15"/>
+      <c r="D12" s="15"/>
+      <c r="E12" s="15"/>
+      <c r="F12" s="15"/>
+      <c r="G12" s="15"/>
+      <c r="H12" s="15"/>
+      <c r="I12" s="15"/>
+      <c r="J12" s="15"/>
+      <c r="K12" s="15"/>
+      <c r="L12" s="15"/>
+      <c r="M12" s="15"/>
+      <c r="N12" s="15"/>
+      <c r="O12" s="15"/>
+      <c r="P12" s="15"/>
+      <c r="Q12" s="15"/>
+      <c r="R12" s="15"/>
+      <c r="S12" s="15"/>
+      <c r="T12" s="15"/>
+      <c r="U12" s="15"/>
+      <c r="V12" s="15"/>
+      <c r="W12" s="15"/>
+      <c r="X12" s="15"/>
+      <c r="Y12" s="15"/>
+      <c r="Z12" s="15"/>
+      <c r="AA12" s="15"/>
+      <c r="AB12" s="15"/>
+      <c r="AC12" s="15"/>
+      <c r="AD12" s="15"/>
+      <c r="AE12" s="15"/>
+      <c r="AF12" s="15"/>
+      <c r="AG12" s="15"/>
+      <c r="AH12" s="15"/>
+      <c r="AI12" s="16"/>
     </row>
     <row r="13" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A13" s="35" t="s">
+      <c r="A13" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="B13" s="35" t="s">
+      <c r="B13" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="C13" s="35"/>
-      <c r="D13" s="35" t="s">
+      <c r="C13" s="17"/>
+      <c r="D13" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="E13" s="35"/>
-      <c r="F13" s="35" t="s">
+      <c r="E13" s="17"/>
+      <c r="F13" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="G13" s="35"/>
-      <c r="H13" s="35"/>
-      <c r="I13" s="35"/>
-      <c r="J13" s="35"/>
-      <c r="K13" s="35"/>
-      <c r="L13" s="35" t="s">
+      <c r="G13" s="17"/>
+      <c r="H13" s="17"/>
+      <c r="I13" s="17"/>
+      <c r="J13" s="17"/>
+      <c r="K13" s="17"/>
+      <c r="L13" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="M13" s="35"/>
-      <c r="N13" s="35" t="s">
+      <c r="M13" s="17"/>
+      <c r="N13" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="O13" s="35"/>
-      <c r="P13" s="35" t="s">
+      <c r="O13" s="17"/>
+      <c r="P13" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="Q13" s="28"/>
-      <c r="R13" s="35" t="s">
+      <c r="Q13" s="18"/>
+      <c r="R13" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="S13" s="35" t="s">
+      <c r="S13" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="T13" s="35"/>
-      <c r="U13" s="35" t="s">
+      <c r="T13" s="17"/>
+      <c r="U13" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="V13" s="35"/>
-      <c r="W13" s="35"/>
-      <c r="X13" s="35" t="s">
+      <c r="V13" s="17"/>
+      <c r="W13" s="17"/>
+      <c r="X13" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="Y13" s="35"/>
-      <c r="Z13" s="35"/>
-      <c r="AA13" s="35"/>
-      <c r="AB13" s="35"/>
-      <c r="AC13" s="35"/>
-      <c r="AD13" s="35" t="s">
+      <c r="Y13" s="17"/>
+      <c r="Z13" s="17"/>
+      <c r="AA13" s="17"/>
+      <c r="AB13" s="17"/>
+      <c r="AC13" s="17"/>
+      <c r="AD13" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="AE13" s="35"/>
-      <c r="AF13" s="35" t="s">
+      <c r="AE13" s="17"/>
+      <c r="AF13" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="AG13" s="35"/>
-      <c r="AH13" s="35" t="s">
+      <c r="AG13" s="17"/>
+      <c r="AH13" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="AI13" s="35"/>
+      <c r="AI13" s="17"/>
     </row>
     <row r="14" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A14" s="35"/>
-      <c r="B14" s="35"/>
-      <c r="C14" s="35"/>
-      <c r="D14" s="35"/>
-      <c r="E14" s="35"/>
-      <c r="F14" s="35"/>
-      <c r="G14" s="35"/>
-      <c r="H14" s="35"/>
-      <c r="I14" s="35"/>
-      <c r="J14" s="35"/>
-      <c r="K14" s="35"/>
-      <c r="L14" s="35"/>
-      <c r="M14" s="35"/>
-      <c r="N14" s="35"/>
-      <c r="O14" s="35"/>
-      <c r="P14" s="28"/>
-      <c r="Q14" s="28"/>
-      <c r="R14" s="35"/>
-      <c r="S14" s="35"/>
-      <c r="T14" s="35"/>
-      <c r="U14" s="35"/>
-      <c r="V14" s="35"/>
-      <c r="W14" s="35"/>
-      <c r="X14" s="35"/>
-      <c r="Y14" s="35"/>
-      <c r="Z14" s="35"/>
-      <c r="AA14" s="35"/>
-      <c r="AB14" s="35"/>
-      <c r="AC14" s="35"/>
-      <c r="AD14" s="35"/>
-      <c r="AE14" s="35"/>
-      <c r="AF14" s="35"/>
-      <c r="AG14" s="35"/>
-      <c r="AH14" s="35"/>
-      <c r="AI14" s="35"/>
+      <c r="A14" s="17"/>
+      <c r="B14" s="17"/>
+      <c r="C14" s="17"/>
+      <c r="D14" s="17"/>
+      <c r="E14" s="17"/>
+      <c r="F14" s="17"/>
+      <c r="G14" s="17"/>
+      <c r="H14" s="17"/>
+      <c r="I14" s="17"/>
+      <c r="J14" s="17"/>
+      <c r="K14" s="17"/>
+      <c r="L14" s="17"/>
+      <c r="M14" s="17"/>
+      <c r="N14" s="17"/>
+      <c r="O14" s="17"/>
+      <c r="P14" s="18"/>
+      <c r="Q14" s="18"/>
+      <c r="R14" s="17"/>
+      <c r="S14" s="17"/>
+      <c r="T14" s="17"/>
+      <c r="U14" s="17"/>
+      <c r="V14" s="17"/>
+      <c r="W14" s="17"/>
+      <c r="X14" s="17"/>
+      <c r="Y14" s="17"/>
+      <c r="Z14" s="17"/>
+      <c r="AA14" s="17"/>
+      <c r="AB14" s="17"/>
+      <c r="AC14" s="17"/>
+      <c r="AD14" s="17"/>
+      <c r="AE14" s="17"/>
+      <c r="AF14" s="17"/>
+      <c r="AG14" s="17"/>
+      <c r="AH14" s="17"/>
+      <c r="AI14" s="17"/>
     </row>
     <row r="15" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A15" s="35"/>
-      <c r="B15" s="35"/>
-      <c r="C15" s="35"/>
-      <c r="D15" s="35"/>
-      <c r="E15" s="35"/>
-      <c r="F15" s="35"/>
-      <c r="G15" s="35"/>
-      <c r="H15" s="35"/>
-      <c r="I15" s="35"/>
-      <c r="J15" s="35"/>
-      <c r="K15" s="35"/>
-      <c r="L15" s="35"/>
-      <c r="M15" s="35"/>
-      <c r="N15" s="35"/>
-      <c r="O15" s="35"/>
-      <c r="P15" s="28"/>
-      <c r="Q15" s="28"/>
-      <c r="R15" s="35"/>
-      <c r="S15" s="35"/>
-      <c r="T15" s="35"/>
-      <c r="U15" s="35"/>
-      <c r="V15" s="35"/>
-      <c r="W15" s="35"/>
-      <c r="X15" s="35"/>
-      <c r="Y15" s="35"/>
-      <c r="Z15" s="35"/>
-      <c r="AA15" s="35"/>
-      <c r="AB15" s="35"/>
-      <c r="AC15" s="35"/>
-      <c r="AD15" s="35"/>
-      <c r="AE15" s="35"/>
-      <c r="AF15" s="35"/>
-      <c r="AG15" s="35"/>
-      <c r="AH15" s="35"/>
-      <c r="AI15" s="35"/>
+      <c r="A15" s="17"/>
+      <c r="B15" s="17"/>
+      <c r="C15" s="17"/>
+      <c r="D15" s="17"/>
+      <c r="E15" s="17"/>
+      <c r="F15" s="17"/>
+      <c r="G15" s="17"/>
+      <c r="H15" s="17"/>
+      <c r="I15" s="17"/>
+      <c r="J15" s="17"/>
+      <c r="K15" s="17"/>
+      <c r="L15" s="17"/>
+      <c r="M15" s="17"/>
+      <c r="N15" s="17"/>
+      <c r="O15" s="17"/>
+      <c r="P15" s="18"/>
+      <c r="Q15" s="18"/>
+      <c r="R15" s="17"/>
+      <c r="S15" s="17"/>
+      <c r="T15" s="17"/>
+      <c r="U15" s="17"/>
+      <c r="V15" s="17"/>
+      <c r="W15" s="17"/>
+      <c r="X15" s="17"/>
+      <c r="Y15" s="17"/>
+      <c r="Z15" s="17"/>
+      <c r="AA15" s="17"/>
+      <c r="AB15" s="17"/>
+      <c r="AC15" s="17"/>
+      <c r="AD15" s="17"/>
+      <c r="AE15" s="17"/>
+      <c r="AF15" s="17"/>
+      <c r="AG15" s="17"/>
+      <c r="AH15" s="17"/>
+      <c r="AI15" s="17"/>
     </row>
     <row r="16" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="7"/>
+      <c r="A16" s="8"/>
       <c r="B16" s="10"/>
       <c r="C16" s="10"/>
-      <c r="D16" s="11"/>
+      <c r="D16" s="12"/>
       <c r="E16" s="10"/>
-      <c r="F16" s="12"/>
-      <c r="G16" s="12"/>
-      <c r="H16" s="12"/>
-      <c r="I16" s="12"/>
-      <c r="J16" s="12"/>
-      <c r="K16" s="12"/>
+      <c r="F16" s="13"/>
+      <c r="G16" s="13"/>
+      <c r="H16" s="13"/>
+      <c r="I16" s="13"/>
+      <c r="J16" s="13"/>
+      <c r="K16" s="13"/>
       <c r="L16" s="10"/>
       <c r="M16" s="10"/>
       <c r="N16" s="10"/>
       <c r="O16" s="10"/>
       <c r="P16" s="10"/>
       <c r="Q16" s="10"/>
-      <c r="R16" s="17" t="s">
+      <c r="R16" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="S16" s="36"/>
-      <c r="T16" s="36"/>
-      <c r="U16" s="36"/>
-      <c r="V16" s="36"/>
-      <c r="W16" s="36"/>
-      <c r="X16" s="36"/>
-      <c r="Y16" s="36"/>
-      <c r="Z16" s="36"/>
-      <c r="AA16" s="36"/>
-      <c r="AB16" s="36"/>
-      <c r="AC16" s="36"/>
-      <c r="AD16" s="19"/>
-      <c r="AE16" s="19"/>
-      <c r="AF16" s="19"/>
-      <c r="AG16" s="19"/>
-      <c r="AH16" s="19"/>
-      <c r="AI16" s="19"/>
+      <c r="S16" s="15"/>
+      <c r="T16" s="15"/>
+      <c r="U16" s="15"/>
+      <c r="V16" s="15"/>
+      <c r="W16" s="15"/>
+      <c r="X16" s="15"/>
+      <c r="Y16" s="15"/>
+      <c r="Z16" s="15"/>
+      <c r="AA16" s="15"/>
+      <c r="AB16" s="15"/>
+      <c r="AC16" s="15"/>
+      <c r="AD16" s="11"/>
+      <c r="AE16" s="11"/>
+      <c r="AF16" s="11"/>
+      <c r="AG16" s="11"/>
+      <c r="AH16" s="11"/>
+      <c r="AI16" s="11"/>
     </row>
     <row r="17" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="3"/>
+      <c r="A17" s="8"/>
       <c r="B17" s="10"/>
       <c r="C17" s="10"/>
-      <c r="D17" s="11"/>
+      <c r="D17" s="12"/>
       <c r="E17" s="10"/>
-      <c r="F17" s="12"/>
-      <c r="G17" s="12"/>
-      <c r="H17" s="12"/>
-      <c r="I17" s="12"/>
-      <c r="J17" s="12"/>
-      <c r="K17" s="12"/>
+      <c r="F17" s="37"/>
+      <c r="G17" s="37"/>
+      <c r="H17" s="37"/>
+      <c r="I17" s="37"/>
+      <c r="J17" s="37"/>
+      <c r="K17" s="37"/>
       <c r="L17" s="10"/>
       <c r="M17" s="10"/>
       <c r="N17" s="10"/>
@@ -1495,12 +1494,12 @@
       <c r="U17" s="10"/>
       <c r="V17" s="10"/>
       <c r="W17" s="10"/>
-      <c r="X17" s="10"/>
-      <c r="Y17" s="10"/>
-      <c r="Z17" s="10"/>
-      <c r="AA17" s="10"/>
-      <c r="AB17" s="10"/>
-      <c r="AC17" s="10"/>
+      <c r="X17" s="13"/>
+      <c r="Y17" s="13"/>
+      <c r="Z17" s="13"/>
+      <c r="AA17" s="13"/>
+      <c r="AB17" s="13"/>
+      <c r="AC17" s="13"/>
       <c r="AD17" s="10"/>
       <c r="AE17" s="10"/>
       <c r="AF17" s="10"/>
@@ -1514,14 +1513,14 @@
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
-      <c r="F18" s="19" t="s">
+      <c r="F18" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="G18" s="19"/>
-      <c r="H18" s="19"/>
-      <c r="I18" s="19"/>
-      <c r="J18" s="19"/>
-      <c r="K18" s="19"/>
+      <c r="G18" s="11"/>
+      <c r="H18" s="11"/>
+      <c r="I18" s="11"/>
+      <c r="J18" s="11"/>
+      <c r="K18" s="11"/>
       <c r="L18" s="10"/>
       <c r="M18" s="10"/>
       <c r="N18" s="10"/>
@@ -1534,14 +1533,14 @@
       <c r="U18" s="10"/>
       <c r="V18" s="10"/>
       <c r="W18" s="10"/>
-      <c r="X18" s="19" t="s">
+      <c r="X18" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="Y18" s="19"/>
-      <c r="Z18" s="19"/>
-      <c r="AA18" s="19"/>
-      <c r="AB18" s="19"/>
-      <c r="AC18" s="19"/>
+      <c r="Y18" s="11"/>
+      <c r="Z18" s="11"/>
+      <c r="AA18" s="11"/>
+      <c r="AB18" s="11"/>
+      <c r="AC18" s="11"/>
       <c r="AD18" s="10"/>
       <c r="AE18" s="10"/>
       <c r="AF18" s="10"/>
@@ -1551,68 +1550,24 @@
     </row>
   </sheetData>
   <mergeCells count="97">
-    <mergeCell ref="H1:Y1"/>
-    <mergeCell ref="U18:W18"/>
-    <mergeCell ref="X18:AC18"/>
-    <mergeCell ref="AD18:AE18"/>
-    <mergeCell ref="AF18:AG18"/>
-    <mergeCell ref="AH18:AI18"/>
-    <mergeCell ref="U10:W10"/>
-    <mergeCell ref="X10:Y10"/>
-    <mergeCell ref="AD17:AE17"/>
-    <mergeCell ref="AF17:AG17"/>
-    <mergeCell ref="AH17:AI17"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="F18:K18"/>
-    <mergeCell ref="L18:M18"/>
-    <mergeCell ref="N18:O18"/>
-    <mergeCell ref="P18:Q18"/>
-    <mergeCell ref="S18:T18"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="F17:K17"/>
-    <mergeCell ref="L17:M17"/>
-    <mergeCell ref="N17:O17"/>
-    <mergeCell ref="P17:Q17"/>
-    <mergeCell ref="S17:T17"/>
-    <mergeCell ref="U17:W17"/>
-    <mergeCell ref="X17:AC17"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="F16:K16"/>
-    <mergeCell ref="L16:M16"/>
-    <mergeCell ref="N16:O16"/>
-    <mergeCell ref="P16:Q16"/>
-    <mergeCell ref="R16:AC16"/>
-    <mergeCell ref="A12:AI12"/>
-    <mergeCell ref="A13:A15"/>
-    <mergeCell ref="B13:C15"/>
-    <mergeCell ref="D13:E15"/>
-    <mergeCell ref="F13:K15"/>
-    <mergeCell ref="L13:M15"/>
-    <mergeCell ref="N13:O15"/>
-    <mergeCell ref="P13:Q15"/>
-    <mergeCell ref="AD16:AE16"/>
-    <mergeCell ref="AF16:AG16"/>
-    <mergeCell ref="AH16:AI16"/>
-    <mergeCell ref="AH13:AI15"/>
-    <mergeCell ref="X13:AC15"/>
-    <mergeCell ref="AD13:AE15"/>
-    <mergeCell ref="AF13:AG15"/>
-    <mergeCell ref="AB11:AC11"/>
-    <mergeCell ref="AB8:AC10"/>
-    <mergeCell ref="Z10:AA10"/>
-    <mergeCell ref="N11:O11"/>
-    <mergeCell ref="P11:Q11"/>
-    <mergeCell ref="R11:T11"/>
-    <mergeCell ref="X11:Y11"/>
-    <mergeCell ref="U11:W11"/>
-    <mergeCell ref="R13:R15"/>
-    <mergeCell ref="S13:T15"/>
-    <mergeCell ref="U13:W15"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="O6:T6"/>
+    <mergeCell ref="AC4:AF4"/>
+    <mergeCell ref="AC5:AF5"/>
+    <mergeCell ref="AC6:AF6"/>
+    <mergeCell ref="A5:H5"/>
+    <mergeCell ref="O5:T5"/>
+    <mergeCell ref="O4:T4"/>
+    <mergeCell ref="K4:N4"/>
+    <mergeCell ref="K5:N5"/>
+    <mergeCell ref="Z4:AB4"/>
+    <mergeCell ref="Z5:AB5"/>
+    <mergeCell ref="A6:H6"/>
+    <mergeCell ref="K6:N6"/>
+    <mergeCell ref="Z6:AB6"/>
+    <mergeCell ref="A11:C11"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="H11:I11"/>
+    <mergeCell ref="J11:K11"/>
     <mergeCell ref="AD11:AG11"/>
     <mergeCell ref="AH11:AI11"/>
     <mergeCell ref="A8:AA9"/>
@@ -1629,25 +1584,69 @@
     <mergeCell ref="R10:T10"/>
     <mergeCell ref="AD8:AG10"/>
     <mergeCell ref="A10:C10"/>
-    <mergeCell ref="A11:C11"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="F11:G11"/>
-    <mergeCell ref="H11:I11"/>
-    <mergeCell ref="J11:K11"/>
+    <mergeCell ref="R13:R15"/>
+    <mergeCell ref="S13:T15"/>
+    <mergeCell ref="U13:W15"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="O6:T6"/>
     <mergeCell ref="L11:M11"/>
-    <mergeCell ref="AC4:AF4"/>
-    <mergeCell ref="AC5:AF5"/>
-    <mergeCell ref="AC6:AF6"/>
-    <mergeCell ref="A5:H5"/>
-    <mergeCell ref="O5:T5"/>
-    <mergeCell ref="O4:T4"/>
-    <mergeCell ref="K4:N4"/>
-    <mergeCell ref="K5:N5"/>
-    <mergeCell ref="Z4:AB4"/>
-    <mergeCell ref="Z5:AB5"/>
-    <mergeCell ref="A6:H6"/>
-    <mergeCell ref="K6:N6"/>
-    <mergeCell ref="Z6:AB6"/>
+    <mergeCell ref="N11:O11"/>
+    <mergeCell ref="P11:Q11"/>
+    <mergeCell ref="R11:T11"/>
+    <mergeCell ref="X11:Y11"/>
+    <mergeCell ref="U11:W11"/>
+    <mergeCell ref="AH16:AI16"/>
+    <mergeCell ref="AH13:AI15"/>
+    <mergeCell ref="X13:AC15"/>
+    <mergeCell ref="AD13:AE15"/>
+    <mergeCell ref="AF13:AG15"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="F16:K16"/>
+    <mergeCell ref="L16:M16"/>
+    <mergeCell ref="N16:O16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="F17:K17"/>
+    <mergeCell ref="L17:M17"/>
+    <mergeCell ref="N17:O17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="F18:K18"/>
+    <mergeCell ref="L18:M18"/>
+    <mergeCell ref="N18:O18"/>
+    <mergeCell ref="AH18:AI18"/>
+    <mergeCell ref="U10:W10"/>
+    <mergeCell ref="X10:Y10"/>
+    <mergeCell ref="AD17:AE17"/>
+    <mergeCell ref="AF17:AG17"/>
+    <mergeCell ref="AH17:AI17"/>
+    <mergeCell ref="U17:W17"/>
+    <mergeCell ref="X17:AC17"/>
+    <mergeCell ref="R16:AC16"/>
+    <mergeCell ref="A12:AI12"/>
+    <mergeCell ref="A13:A15"/>
+    <mergeCell ref="B13:C15"/>
+    <mergeCell ref="D13:E15"/>
+    <mergeCell ref="F13:K15"/>
+    <mergeCell ref="L13:M15"/>
+    <mergeCell ref="N13:O15"/>
+    <mergeCell ref="H1:Y1"/>
+    <mergeCell ref="U18:W18"/>
+    <mergeCell ref="X18:AC18"/>
+    <mergeCell ref="AD18:AE18"/>
+    <mergeCell ref="AF18:AG18"/>
+    <mergeCell ref="P18:Q18"/>
+    <mergeCell ref="S18:T18"/>
+    <mergeCell ref="P17:Q17"/>
+    <mergeCell ref="S17:T17"/>
+    <mergeCell ref="P16:Q16"/>
+    <mergeCell ref="P13:Q15"/>
+    <mergeCell ref="AD16:AE16"/>
+    <mergeCell ref="AF16:AG16"/>
+    <mergeCell ref="AB11:AC11"/>
+    <mergeCell ref="AB8:AC10"/>
+    <mergeCell ref="Z10:AA10"/>
   </mergeCells>
   <pageMargins left="0.22159090909090901" right="0.2" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="65" orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
tinggal cek keluar masuk barang
</commit_message>
<xml_diff>
--- a/application/libraries/excel/template - Copy.xlsx
+++ b/application/libraries/excel/template - Copy.xlsx
@@ -15,10 +15,9 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$1:$15</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="0">Sheet1!$1:$15</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
-  <fileRecoveryPr repairLoad="1"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -354,7 +353,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -370,36 +369,74 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="15" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -418,41 +455,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -735,8 +737,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AI18"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" zoomScale="70" zoomScaleNormal="55" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="O19" sqref="O19"/>
+    <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="V27" sqref="V27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -764,26 +766,26 @@
       <c r="E1" s="7"/>
       <c r="F1" s="7"/>
       <c r="G1" s="7"/>
-      <c r="H1" s="9" t="s">
+      <c r="H1" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="I1" s="9"/>
-      <c r="J1" s="9"/>
-      <c r="K1" s="9"/>
-      <c r="L1" s="9"/>
-      <c r="M1" s="9"/>
-      <c r="N1" s="9"/>
-      <c r="O1" s="9"/>
-      <c r="P1" s="9"/>
-      <c r="Q1" s="9"/>
-      <c r="R1" s="9"/>
-      <c r="S1" s="9"/>
-      <c r="T1" s="9"/>
-      <c r="U1" s="9"/>
-      <c r="V1" s="9"/>
-      <c r="W1" s="9"/>
-      <c r="X1" s="9"/>
-      <c r="Y1" s="9"/>
+      <c r="I1" s="32"/>
+      <c r="J1" s="32"/>
+      <c r="K1" s="32"/>
+      <c r="L1" s="32"/>
+      <c r="M1" s="32"/>
+      <c r="N1" s="32"/>
+      <c r="O1" s="32"/>
+      <c r="P1" s="32"/>
+      <c r="Q1" s="32"/>
+      <c r="R1" s="32"/>
+      <c r="S1" s="32"/>
+      <c r="T1" s="32"/>
+      <c r="U1" s="32"/>
+      <c r="V1" s="32"/>
+      <c r="W1" s="32"/>
+      <c r="X1" s="32"/>
+      <c r="Y1" s="32"/>
       <c r="Z1" s="7"/>
       <c r="AA1" s="7"/>
       <c r="AB1" s="7"/>
@@ -880,128 +882,128 @@
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
-      <c r="K4" s="25" t="s">
+      <c r="K4" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="L4" s="25"/>
-      <c r="M4" s="25"/>
-      <c r="N4" s="25"/>
-      <c r="O4" s="25" t="s">
+      <c r="L4" s="10"/>
+      <c r="M4" s="10"/>
+      <c r="N4" s="10"/>
+      <c r="O4" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="P4" s="25"/>
-      <c r="Q4" s="25"/>
-      <c r="R4" s="25"/>
-      <c r="S4" s="25"/>
-      <c r="T4" s="25"/>
+      <c r="P4" s="10"/>
+      <c r="Q4" s="10"/>
+      <c r="R4" s="10"/>
+      <c r="S4" s="10"/>
+      <c r="T4" s="10"/>
       <c r="U4" s="1"/>
       <c r="V4" s="1"/>
       <c r="W4" s="1"/>
       <c r="X4" s="1"/>
       <c r="Y4" s="1"/>
-      <c r="Z4" s="25" t="s">
+      <c r="Z4" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="AA4" s="25"/>
-      <c r="AB4" s="25"/>
-      <c r="AC4" s="25" t="s">
+      <c r="AA4" s="10"/>
+      <c r="AB4" s="10"/>
+      <c r="AC4" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="AD4" s="25"/>
-      <c r="AE4" s="25"/>
-      <c r="AF4" s="25"/>
+      <c r="AD4" s="10"/>
+      <c r="AE4" s="10"/>
+      <c r="AF4" s="10"/>
       <c r="AG4" s="6"/>
       <c r="AH4" s="6"/>
       <c r="AI4" s="6"/>
     </row>
     <row r="5" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="34" t="s">
+      <c r="A5" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="34"/>
-      <c r="C5" s="34"/>
-      <c r="D5" s="34"/>
-      <c r="E5" s="34"/>
-      <c r="F5" s="34"/>
-      <c r="G5" s="34"/>
-      <c r="H5" s="34"/>
+      <c r="B5" s="11"/>
+      <c r="C5" s="11"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="11"/>
+      <c r="F5" s="11"/>
+      <c r="G5" s="11"/>
+      <c r="H5" s="11"/>
       <c r="I5" s="4"/>
       <c r="J5" s="2"/>
-      <c r="K5" s="25" t="s">
+      <c r="K5" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="L5" s="25"/>
-      <c r="M5" s="25"/>
-      <c r="N5" s="25"/>
-      <c r="O5" s="35" t="s">
+      <c r="L5" s="10"/>
+      <c r="M5" s="10"/>
+      <c r="N5" s="10"/>
+      <c r="O5" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="P5" s="35"/>
-      <c r="Q5" s="35"/>
-      <c r="R5" s="35"/>
-      <c r="S5" s="35"/>
-      <c r="T5" s="35"/>
+      <c r="P5" s="12"/>
+      <c r="Q5" s="12"/>
+      <c r="R5" s="12"/>
+      <c r="S5" s="12"/>
+      <c r="T5" s="12"/>
       <c r="U5" s="1"/>
       <c r="V5" s="1"/>
       <c r="W5" s="1"/>
       <c r="X5" s="1"/>
       <c r="Y5" s="1"/>
-      <c r="Z5" s="36" t="s">
+      <c r="Z5" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="AA5" s="36"/>
-      <c r="AB5" s="36"/>
-      <c r="AC5" s="25" t="s">
+      <c r="AA5" s="13"/>
+      <c r="AB5" s="13"/>
+      <c r="AC5" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="AD5" s="25"/>
-      <c r="AE5" s="25"/>
-      <c r="AF5" s="25"/>
+      <c r="AD5" s="10"/>
+      <c r="AE5" s="10"/>
+      <c r="AF5" s="10"/>
       <c r="AG5" s="6"/>
       <c r="AH5" s="6"/>
       <c r="AI5" s="6"/>
     </row>
     <row r="6" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="34"/>
-      <c r="B6" s="34"/>
-      <c r="C6" s="34"/>
-      <c r="D6" s="34"/>
-      <c r="E6" s="34"/>
-      <c r="F6" s="34"/>
-      <c r="G6" s="34"/>
-      <c r="H6" s="34"/>
+      <c r="A6" s="11"/>
+      <c r="B6" s="11"/>
+      <c r="C6" s="11"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="11"/>
+      <c r="G6" s="11"/>
+      <c r="H6" s="11"/>
       <c r="I6" s="4"/>
       <c r="J6" s="2"/>
-      <c r="K6" s="25" t="s">
+      <c r="K6" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="L6" s="25"/>
-      <c r="M6" s="25"/>
-      <c r="N6" s="25"/>
-      <c r="O6" s="25" t="s">
+      <c r="L6" s="10"/>
+      <c r="M6" s="10"/>
+      <c r="N6" s="10"/>
+      <c r="O6" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="P6" s="25"/>
-      <c r="Q6" s="25"/>
-      <c r="R6" s="25"/>
-      <c r="S6" s="25"/>
-      <c r="T6" s="25"/>
+      <c r="P6" s="10"/>
+      <c r="Q6" s="10"/>
+      <c r="R6" s="10"/>
+      <c r="S6" s="10"/>
+      <c r="T6" s="10"/>
       <c r="U6" s="1"/>
       <c r="V6" s="1"/>
       <c r="W6" s="1"/>
       <c r="X6" s="1"/>
       <c r="Y6" s="1"/>
-      <c r="Z6" s="25" t="s">
+      <c r="Z6" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="AA6" s="25"/>
-      <c r="AB6" s="25"/>
-      <c r="AC6" s="25" t="s">
+      <c r="AA6" s="10"/>
+      <c r="AB6" s="10"/>
+      <c r="AC6" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="AD6" s="25"/>
-      <c r="AE6" s="25"/>
-      <c r="AF6" s="25"/>
+      <c r="AD6" s="10"/>
+      <c r="AE6" s="10"/>
+      <c r="AF6" s="10"/>
       <c r="AG6" s="6"/>
       <c r="AH6" s="6"/>
       <c r="AI6" s="5"/>
@@ -1017,25 +1019,25 @@
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
-      <c r="K7" s="32" t="s">
+      <c r="K7" s="21" t="s">
         <v>40</v>
       </c>
-      <c r="L7" s="32"/>
-      <c r="M7" s="32"/>
-      <c r="N7" s="32"/>
-      <c r="O7" s="32" t="s">
+      <c r="L7" s="21"/>
+      <c r="M7" s="21"/>
+      <c r="N7" s="21"/>
+      <c r="O7" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="P7" s="32"/>
-      <c r="Q7" s="32"/>
-      <c r="R7" s="32"/>
-      <c r="S7" s="32"/>
-      <c r="T7" s="32"/>
-      <c r="U7" s="32"/>
-      <c r="V7" s="32"/>
-      <c r="W7" s="32"/>
-      <c r="X7" s="32"/>
-      <c r="Y7" s="32"/>
+      <c r="P7" s="21"/>
+      <c r="Q7" s="21"/>
+      <c r="R7" s="21"/>
+      <c r="S7" s="21"/>
+      <c r="T7" s="21"/>
+      <c r="U7" s="21"/>
+      <c r="V7" s="21"/>
+      <c r="W7" s="21"/>
+      <c r="X7" s="21"/>
+      <c r="Y7" s="21"/>
       <c r="Z7" s="1"/>
       <c r="AA7" s="1"/>
       <c r="AB7" s="1"/>
@@ -1048,526 +1050,571 @@
       <c r="AI7" s="5"/>
     </row>
     <row r="8" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="26" t="s">
+      <c r="A8" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="27"/>
-      <c r="C8" s="27"/>
-      <c r="D8" s="27"/>
-      <c r="E8" s="27"/>
-      <c r="F8" s="27"/>
-      <c r="G8" s="27"/>
-      <c r="H8" s="27"/>
-      <c r="I8" s="27"/>
-      <c r="J8" s="27"/>
-      <c r="K8" s="27"/>
-      <c r="L8" s="27"/>
-      <c r="M8" s="27"/>
-      <c r="N8" s="27"/>
-      <c r="O8" s="27"/>
-      <c r="P8" s="27"/>
-      <c r="Q8" s="27"/>
-      <c r="R8" s="27"/>
-      <c r="S8" s="27"/>
-      <c r="T8" s="27"/>
-      <c r="U8" s="27"/>
-      <c r="V8" s="27"/>
-      <c r="W8" s="27"/>
-      <c r="X8" s="27"/>
-      <c r="Y8" s="27"/>
-      <c r="Z8" s="27"/>
-      <c r="AA8" s="28"/>
-      <c r="AB8" s="19" t="s">
+      <c r="B8" s="16"/>
+      <c r="C8" s="16"/>
+      <c r="D8" s="16"/>
+      <c r="E8" s="16"/>
+      <c r="F8" s="16"/>
+      <c r="G8" s="16"/>
+      <c r="H8" s="16"/>
+      <c r="I8" s="16"/>
+      <c r="J8" s="16"/>
+      <c r="K8" s="16"/>
+      <c r="L8" s="16"/>
+      <c r="M8" s="16"/>
+      <c r="N8" s="16"/>
+      <c r="O8" s="16"/>
+      <c r="P8" s="16"/>
+      <c r="Q8" s="16"/>
+      <c r="R8" s="16"/>
+      <c r="S8" s="16"/>
+      <c r="T8" s="16"/>
+      <c r="U8" s="16"/>
+      <c r="V8" s="16"/>
+      <c r="W8" s="16"/>
+      <c r="X8" s="16"/>
+      <c r="Y8" s="16"/>
+      <c r="Z8" s="16"/>
+      <c r="AA8" s="17"/>
+      <c r="AB8" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="AC8" s="20"/>
-      <c r="AD8" s="33" t="s">
+      <c r="AC8" s="34"/>
+      <c r="AD8" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="AE8" s="33"/>
-      <c r="AF8" s="33"/>
-      <c r="AG8" s="33"/>
-      <c r="AH8" s="33" t="s">
+      <c r="AE8" s="24"/>
+      <c r="AF8" s="24"/>
+      <c r="AG8" s="24"/>
+      <c r="AH8" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="AI8" s="33"/>
+      <c r="AI8" s="24"/>
     </row>
     <row r="9" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="29"/>
-      <c r="B9" s="30"/>
-      <c r="C9" s="30"/>
-      <c r="D9" s="30"/>
-      <c r="E9" s="30"/>
-      <c r="F9" s="30"/>
-      <c r="G9" s="30"/>
-      <c r="H9" s="30"/>
-      <c r="I9" s="30"/>
-      <c r="J9" s="30"/>
-      <c r="K9" s="30"/>
-      <c r="L9" s="30"/>
-      <c r="M9" s="30"/>
-      <c r="N9" s="30"/>
-      <c r="O9" s="30"/>
-      <c r="P9" s="30"/>
-      <c r="Q9" s="30"/>
-      <c r="R9" s="30"/>
-      <c r="S9" s="30"/>
-      <c r="T9" s="30"/>
-      <c r="U9" s="30"/>
-      <c r="V9" s="30"/>
-      <c r="W9" s="30"/>
-      <c r="X9" s="30"/>
-      <c r="Y9" s="30"/>
-      <c r="Z9" s="30"/>
-      <c r="AA9" s="31"/>
-      <c r="AB9" s="21"/>
-      <c r="AC9" s="22"/>
-      <c r="AD9" s="33"/>
-      <c r="AE9" s="33"/>
-      <c r="AF9" s="33"/>
-      <c r="AG9" s="33"/>
-      <c r="AH9" s="33"/>
-      <c r="AI9" s="33"/>
+      <c r="A9" s="18"/>
+      <c r="B9" s="19"/>
+      <c r="C9" s="19"/>
+      <c r="D9" s="19"/>
+      <c r="E9" s="19"/>
+      <c r="F9" s="19"/>
+      <c r="G9" s="19"/>
+      <c r="H9" s="19"/>
+      <c r="I9" s="19"/>
+      <c r="J9" s="19"/>
+      <c r="K9" s="19"/>
+      <c r="L9" s="19"/>
+      <c r="M9" s="19"/>
+      <c r="N9" s="19"/>
+      <c r="O9" s="19"/>
+      <c r="P9" s="19"/>
+      <c r="Q9" s="19"/>
+      <c r="R9" s="19"/>
+      <c r="S9" s="19"/>
+      <c r="T9" s="19"/>
+      <c r="U9" s="19"/>
+      <c r="V9" s="19"/>
+      <c r="W9" s="19"/>
+      <c r="X9" s="19"/>
+      <c r="Y9" s="19"/>
+      <c r="Z9" s="19"/>
+      <c r="AA9" s="20"/>
+      <c r="AB9" s="35"/>
+      <c r="AC9" s="36"/>
+      <c r="AD9" s="24"/>
+      <c r="AE9" s="24"/>
+      <c r="AF9" s="24"/>
+      <c r="AG9" s="24"/>
+      <c r="AH9" s="24"/>
+      <c r="AI9" s="24"/>
     </row>
     <row r="10" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="11" t="s">
+      <c r="A10" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="11"/>
-      <c r="C10" s="11"/>
-      <c r="D10" s="14" t="s">
+      <c r="B10" s="14"/>
+      <c r="C10" s="14"/>
+      <c r="D10" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="E10" s="16"/>
-      <c r="F10" s="11" t="s">
+      <c r="E10" s="23"/>
+      <c r="F10" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="G10" s="11"/>
-      <c r="H10" s="11" t="s">
+      <c r="G10" s="14"/>
+      <c r="H10" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="I10" s="11"/>
-      <c r="J10" s="11" t="s">
+      <c r="I10" s="14"/>
+      <c r="J10" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="K10" s="11"/>
-      <c r="L10" s="11" t="s">
+      <c r="K10" s="14"/>
+      <c r="L10" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="M10" s="11"/>
-      <c r="N10" s="11" t="s">
+      <c r="M10" s="14"/>
+      <c r="N10" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="O10" s="18"/>
-      <c r="P10" s="11" t="s">
+      <c r="O10" s="25"/>
+      <c r="P10" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="Q10" s="11"/>
-      <c r="R10" s="11" t="s">
+      <c r="Q10" s="14"/>
+      <c r="R10" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="S10" s="11"/>
-      <c r="T10" s="11"/>
-      <c r="U10" s="11" t="s">
+      <c r="S10" s="14"/>
+      <c r="T10" s="14"/>
+      <c r="U10" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="V10" s="11"/>
-      <c r="W10" s="11"/>
-      <c r="X10" s="11" t="s">
+      <c r="V10" s="14"/>
+      <c r="W10" s="14"/>
+      <c r="X10" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="Y10" s="11"/>
-      <c r="Z10" s="14" t="s">
+      <c r="Y10" s="14"/>
+      <c r="Z10" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="AA10" s="16"/>
-      <c r="AB10" s="23"/>
-      <c r="AC10" s="24"/>
-      <c r="AD10" s="33"/>
-      <c r="AE10" s="33"/>
-      <c r="AF10" s="33"/>
-      <c r="AG10" s="33"/>
-      <c r="AH10" s="33"/>
-      <c r="AI10" s="33"/>
+      <c r="AA10" s="23"/>
+      <c r="AB10" s="37"/>
+      <c r="AC10" s="38"/>
+      <c r="AD10" s="24"/>
+      <c r="AE10" s="24"/>
+      <c r="AF10" s="24"/>
+      <c r="AG10" s="24"/>
+      <c r="AH10" s="24"/>
+      <c r="AI10" s="24"/>
     </row>
     <row r="11" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="11">
+      <c r="A11" s="14">
         <v>0</v>
       </c>
-      <c r="B11" s="11"/>
-      <c r="C11" s="11"/>
-      <c r="D11" s="11">
+      <c r="B11" s="14"/>
+      <c r="C11" s="14"/>
+      <c r="D11" s="14">
         <v>0</v>
       </c>
-      <c r="E11" s="11"/>
-      <c r="F11" s="11">
+      <c r="E11" s="14"/>
+      <c r="F11" s="14">
         <v>0</v>
       </c>
-      <c r="G11" s="11"/>
-      <c r="H11" s="11">
+      <c r="G11" s="14"/>
+      <c r="H11" s="14">
         <v>0</v>
       </c>
-      <c r="I11" s="11"/>
-      <c r="J11" s="11">
+      <c r="I11" s="14"/>
+      <c r="J11" s="14">
         <v>0</v>
       </c>
-      <c r="K11" s="11"/>
-      <c r="L11" s="11">
+      <c r="K11" s="14"/>
+      <c r="L11" s="14">
         <v>0</v>
       </c>
-      <c r="M11" s="11"/>
-      <c r="N11" s="11">
+      <c r="M11" s="14"/>
+      <c r="N11" s="14">
         <v>0</v>
       </c>
-      <c r="O11" s="11"/>
-      <c r="P11" s="11">
+      <c r="O11" s="14"/>
+      <c r="P11" s="14">
         <v>0</v>
       </c>
-      <c r="Q11" s="11"/>
-      <c r="R11" s="11">
+      <c r="Q11" s="14"/>
+      <c r="R11" s="14">
         <v>0</v>
       </c>
-      <c r="S11" s="11"/>
-      <c r="T11" s="11"/>
-      <c r="U11" s="11">
+      <c r="S11" s="14"/>
+      <c r="T11" s="14"/>
+      <c r="U11" s="14">
         <v>0</v>
       </c>
-      <c r="V11" s="11"/>
-      <c r="W11" s="11"/>
-      <c r="X11" s="11">
+      <c r="V11" s="14"/>
+      <c r="W11" s="14"/>
+      <c r="X11" s="14">
         <v>0</v>
       </c>
-      <c r="Y11" s="11"/>
-      <c r="Z11" s="14">
+      <c r="Y11" s="14"/>
+      <c r="Z11" s="22">
         <v>0</v>
       </c>
-      <c r="AA11" s="16"/>
-      <c r="AB11" s="14"/>
-      <c r="AC11" s="16"/>
-      <c r="AD11" s="11">
+      <c r="AA11" s="23"/>
+      <c r="AB11" s="22"/>
+      <c r="AC11" s="23"/>
+      <c r="AD11" s="14">
         <v>0</v>
       </c>
-      <c r="AE11" s="11"/>
-      <c r="AF11" s="11"/>
-      <c r="AG11" s="11"/>
-      <c r="AH11" s="11">
+      <c r="AE11" s="14"/>
+      <c r="AF11" s="14"/>
+      <c r="AG11" s="14"/>
+      <c r="AH11" s="14">
         <v>0</v>
       </c>
-      <c r="AI11" s="11"/>
+      <c r="AI11" s="14"/>
     </row>
     <row r="12" spans="1:35" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="14"/>
-      <c r="B12" s="15"/>
-      <c r="C12" s="15"/>
-      <c r="D12" s="15"/>
-      <c r="E12" s="15"/>
-      <c r="F12" s="15"/>
-      <c r="G12" s="15"/>
-      <c r="H12" s="15"/>
-      <c r="I12" s="15"/>
-      <c r="J12" s="15"/>
-      <c r="K12" s="15"/>
-      <c r="L12" s="15"/>
-      <c r="M12" s="15"/>
-      <c r="N12" s="15"/>
-      <c r="O12" s="15"/>
-      <c r="P12" s="15"/>
-      <c r="Q12" s="15"/>
-      <c r="R12" s="15"/>
-      <c r="S12" s="15"/>
-      <c r="T12" s="15"/>
-      <c r="U12" s="15"/>
-      <c r="V12" s="15"/>
-      <c r="W12" s="15"/>
-      <c r="X12" s="15"/>
-      <c r="Y12" s="15"/>
-      <c r="Z12" s="15"/>
-      <c r="AA12" s="15"/>
-      <c r="AB12" s="15"/>
-      <c r="AC12" s="15"/>
-      <c r="AD12" s="15"/>
-      <c r="AE12" s="15"/>
-      <c r="AF12" s="15"/>
-      <c r="AG12" s="15"/>
-      <c r="AH12" s="15"/>
-      <c r="AI12" s="16"/>
+      <c r="A12" s="22"/>
+      <c r="B12" s="31"/>
+      <c r="C12" s="31"/>
+      <c r="D12" s="31"/>
+      <c r="E12" s="31"/>
+      <c r="F12" s="31"/>
+      <c r="G12" s="31"/>
+      <c r="H12" s="31"/>
+      <c r="I12" s="31"/>
+      <c r="J12" s="31"/>
+      <c r="K12" s="31"/>
+      <c r="L12" s="31"/>
+      <c r="M12" s="31"/>
+      <c r="N12" s="31"/>
+      <c r="O12" s="31"/>
+      <c r="P12" s="31"/>
+      <c r="Q12" s="31"/>
+      <c r="R12" s="31"/>
+      <c r="S12" s="31"/>
+      <c r="T12" s="31"/>
+      <c r="U12" s="31"/>
+      <c r="V12" s="31"/>
+      <c r="W12" s="31"/>
+      <c r="X12" s="31"/>
+      <c r="Y12" s="31"/>
+      <c r="Z12" s="31"/>
+      <c r="AA12" s="31"/>
+      <c r="AB12" s="31"/>
+      <c r="AC12" s="31"/>
+      <c r="AD12" s="31"/>
+      <c r="AE12" s="31"/>
+      <c r="AF12" s="31"/>
+      <c r="AG12" s="31"/>
+      <c r="AH12" s="31"/>
+      <c r="AI12" s="23"/>
     </row>
     <row r="13" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A13" s="17" t="s">
+      <c r="A13" s="26" t="s">
         <v>35</v>
       </c>
-      <c r="B13" s="17" t="s">
+      <c r="B13" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="C13" s="17"/>
-      <c r="D13" s="17" t="s">
+      <c r="C13" s="26"/>
+      <c r="D13" s="26" t="s">
         <v>26</v>
       </c>
-      <c r="E13" s="17"/>
-      <c r="F13" s="17" t="s">
+      <c r="E13" s="26"/>
+      <c r="F13" s="26" t="s">
         <v>27</v>
       </c>
-      <c r="G13" s="17"/>
-      <c r="H13" s="17"/>
-      <c r="I13" s="17"/>
-      <c r="J13" s="17"/>
-      <c r="K13" s="17"/>
-      <c r="L13" s="17" t="s">
+      <c r="G13" s="26"/>
+      <c r="H13" s="26"/>
+      <c r="I13" s="26"/>
+      <c r="J13" s="26"/>
+      <c r="K13" s="26"/>
+      <c r="L13" s="26" t="s">
         <v>28</v>
       </c>
-      <c r="M13" s="17"/>
-      <c r="N13" s="17" t="s">
+      <c r="M13" s="26"/>
+      <c r="N13" s="26" t="s">
         <v>29</v>
       </c>
-      <c r="O13" s="17"/>
-      <c r="P13" s="17" t="s">
+      <c r="O13" s="26"/>
+      <c r="P13" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="Q13" s="18"/>
-      <c r="R13" s="17" t="s">
+      <c r="Q13" s="25"/>
+      <c r="R13" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="S13" s="17" t="s">
+      <c r="S13" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="T13" s="17"/>
-      <c r="U13" s="17" t="s">
+      <c r="T13" s="26"/>
+      <c r="U13" s="26" t="s">
         <v>26</v>
       </c>
-      <c r="V13" s="17"/>
-      <c r="W13" s="17"/>
-      <c r="X13" s="17" t="s">
+      <c r="V13" s="26"/>
+      <c r="W13" s="26"/>
+      <c r="X13" s="26" t="s">
         <v>27</v>
       </c>
-      <c r="Y13" s="17"/>
-      <c r="Z13" s="17"/>
-      <c r="AA13" s="17"/>
-      <c r="AB13" s="17"/>
-      <c r="AC13" s="17"/>
-      <c r="AD13" s="17" t="s">
+      <c r="Y13" s="26"/>
+      <c r="Z13" s="26"/>
+      <c r="AA13" s="26"/>
+      <c r="AB13" s="26"/>
+      <c r="AC13" s="26"/>
+      <c r="AD13" s="26" t="s">
         <v>31</v>
       </c>
-      <c r="AE13" s="17"/>
-      <c r="AF13" s="17" t="s">
+      <c r="AE13" s="26"/>
+      <c r="AF13" s="26" t="s">
         <v>29</v>
       </c>
-      <c r="AG13" s="17"/>
-      <c r="AH13" s="17" t="s">
+      <c r="AG13" s="26"/>
+      <c r="AH13" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="AI13" s="17"/>
+      <c r="AI13" s="26"/>
     </row>
     <row r="14" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A14" s="17"/>
-      <c r="B14" s="17"/>
-      <c r="C14" s="17"/>
-      <c r="D14" s="17"/>
-      <c r="E14" s="17"/>
-      <c r="F14" s="17"/>
-      <c r="G14" s="17"/>
-      <c r="H14" s="17"/>
-      <c r="I14" s="17"/>
-      <c r="J14" s="17"/>
-      <c r="K14" s="17"/>
-      <c r="L14" s="17"/>
-      <c r="M14" s="17"/>
-      <c r="N14" s="17"/>
-      <c r="O14" s="17"/>
-      <c r="P14" s="18"/>
-      <c r="Q14" s="18"/>
-      <c r="R14" s="17"/>
-      <c r="S14" s="17"/>
-      <c r="T14" s="17"/>
-      <c r="U14" s="17"/>
-      <c r="V14" s="17"/>
-      <c r="W14" s="17"/>
-      <c r="X14" s="17"/>
-      <c r="Y14" s="17"/>
-      <c r="Z14" s="17"/>
-      <c r="AA14" s="17"/>
-      <c r="AB14" s="17"/>
-      <c r="AC14" s="17"/>
-      <c r="AD14" s="17"/>
-      <c r="AE14" s="17"/>
-      <c r="AF14" s="17"/>
-      <c r="AG14" s="17"/>
-      <c r="AH14" s="17"/>
-      <c r="AI14" s="17"/>
+      <c r="A14" s="26"/>
+      <c r="B14" s="26"/>
+      <c r="C14" s="26"/>
+      <c r="D14" s="26"/>
+      <c r="E14" s="26"/>
+      <c r="F14" s="26"/>
+      <c r="G14" s="26"/>
+      <c r="H14" s="26"/>
+      <c r="I14" s="26"/>
+      <c r="J14" s="26"/>
+      <c r="K14" s="26"/>
+      <c r="L14" s="26"/>
+      <c r="M14" s="26"/>
+      <c r="N14" s="26"/>
+      <c r="O14" s="26"/>
+      <c r="P14" s="25"/>
+      <c r="Q14" s="25"/>
+      <c r="R14" s="26"/>
+      <c r="S14" s="26"/>
+      <c r="T14" s="26"/>
+      <c r="U14" s="26"/>
+      <c r="V14" s="26"/>
+      <c r="W14" s="26"/>
+      <c r="X14" s="26"/>
+      <c r="Y14" s="26"/>
+      <c r="Z14" s="26"/>
+      <c r="AA14" s="26"/>
+      <c r="AB14" s="26"/>
+      <c r="AC14" s="26"/>
+      <c r="AD14" s="26"/>
+      <c r="AE14" s="26"/>
+      <c r="AF14" s="26"/>
+      <c r="AG14" s="26"/>
+      <c r="AH14" s="26"/>
+      <c r="AI14" s="26"/>
     </row>
     <row r="15" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A15" s="17"/>
-      <c r="B15" s="17"/>
-      <c r="C15" s="17"/>
-      <c r="D15" s="17"/>
-      <c r="E15" s="17"/>
-      <c r="F15" s="17"/>
-      <c r="G15" s="17"/>
-      <c r="H15" s="17"/>
-      <c r="I15" s="17"/>
-      <c r="J15" s="17"/>
-      <c r="K15" s="17"/>
-      <c r="L15" s="17"/>
-      <c r="M15" s="17"/>
-      <c r="N15" s="17"/>
-      <c r="O15" s="17"/>
-      <c r="P15" s="18"/>
-      <c r="Q15" s="18"/>
-      <c r="R15" s="17"/>
-      <c r="S15" s="17"/>
-      <c r="T15" s="17"/>
-      <c r="U15" s="17"/>
-      <c r="V15" s="17"/>
-      <c r="W15" s="17"/>
-      <c r="X15" s="17"/>
-      <c r="Y15" s="17"/>
-      <c r="Z15" s="17"/>
-      <c r="AA15" s="17"/>
-      <c r="AB15" s="17"/>
-      <c r="AC15" s="17"/>
-      <c r="AD15" s="17"/>
-      <c r="AE15" s="17"/>
-      <c r="AF15" s="17"/>
-      <c r="AG15" s="17"/>
-      <c r="AH15" s="17"/>
-      <c r="AI15" s="17"/>
+      <c r="A15" s="26"/>
+      <c r="B15" s="26"/>
+      <c r="C15" s="26"/>
+      <c r="D15" s="26"/>
+      <c r="E15" s="26"/>
+      <c r="F15" s="26"/>
+      <c r="G15" s="26"/>
+      <c r="H15" s="26"/>
+      <c r="I15" s="26"/>
+      <c r="J15" s="26"/>
+      <c r="K15" s="26"/>
+      <c r="L15" s="26"/>
+      <c r="M15" s="26"/>
+      <c r="N15" s="26"/>
+      <c r="O15" s="26"/>
+      <c r="P15" s="25"/>
+      <c r="Q15" s="25"/>
+      <c r="R15" s="26"/>
+      <c r="S15" s="26"/>
+      <c r="T15" s="26"/>
+      <c r="U15" s="26"/>
+      <c r="V15" s="26"/>
+      <c r="W15" s="26"/>
+      <c r="X15" s="26"/>
+      <c r="Y15" s="26"/>
+      <c r="Z15" s="26"/>
+      <c r="AA15" s="26"/>
+      <c r="AB15" s="26"/>
+      <c r="AC15" s="26"/>
+      <c r="AD15" s="26"/>
+      <c r="AE15" s="26"/>
+      <c r="AF15" s="26"/>
+      <c r="AG15" s="26"/>
+      <c r="AH15" s="26"/>
+      <c r="AI15" s="26"/>
     </row>
     <row r="16" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="8"/>
-      <c r="B16" s="10"/>
-      <c r="C16" s="10"/>
-      <c r="D16" s="12"/>
-      <c r="E16" s="10"/>
-      <c r="F16" s="13"/>
-      <c r="G16" s="13"/>
-      <c r="H16" s="13"/>
-      <c r="I16" s="13"/>
-      <c r="J16" s="13"/>
-      <c r="K16" s="13"/>
-      <c r="L16" s="10"/>
-      <c r="M16" s="10"/>
-      <c r="N16" s="10"/>
-      <c r="O16" s="10"/>
-      <c r="P16" s="10"/>
-      <c r="Q16" s="10"/>
-      <c r="R16" s="14" t="s">
+      <c r="A16" s="9"/>
+      <c r="B16" s="27"/>
+      <c r="C16" s="27"/>
+      <c r="D16" s="28"/>
+      <c r="E16" s="27"/>
+      <c r="F16" s="29"/>
+      <c r="G16" s="29"/>
+      <c r="H16" s="29"/>
+      <c r="I16" s="29"/>
+      <c r="J16" s="29"/>
+      <c r="K16" s="29"/>
+      <c r="L16" s="27"/>
+      <c r="M16" s="27"/>
+      <c r="N16" s="27"/>
+      <c r="O16" s="27"/>
+      <c r="P16" s="27"/>
+      <c r="Q16" s="27"/>
+      <c r="R16" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="S16" s="15"/>
-      <c r="T16" s="15"/>
-      <c r="U16" s="15"/>
-      <c r="V16" s="15"/>
-      <c r="W16" s="15"/>
-      <c r="X16" s="15"/>
-      <c r="Y16" s="15"/>
-      <c r="Z16" s="15"/>
-      <c r="AA16" s="15"/>
-      <c r="AB16" s="15"/>
-      <c r="AC16" s="15"/>
-      <c r="AD16" s="11"/>
-      <c r="AE16" s="11"/>
-      <c r="AF16" s="11"/>
-      <c r="AG16" s="11"/>
-      <c r="AH16" s="11"/>
-      <c r="AI16" s="11"/>
+      <c r="S16" s="31"/>
+      <c r="T16" s="31"/>
+      <c r="U16" s="31"/>
+      <c r="V16" s="31"/>
+      <c r="W16" s="31"/>
+      <c r="X16" s="31"/>
+      <c r="Y16" s="31"/>
+      <c r="Z16" s="31"/>
+      <c r="AA16" s="31"/>
+      <c r="AB16" s="31"/>
+      <c r="AC16" s="31"/>
+      <c r="AD16" s="14"/>
+      <c r="AE16" s="14"/>
+      <c r="AF16" s="14"/>
+      <c r="AG16" s="14"/>
+      <c r="AH16" s="14"/>
+      <c r="AI16" s="14"/>
     </row>
     <row r="17" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="8"/>
-      <c r="B17" s="10"/>
-      <c r="C17" s="10"/>
-      <c r="D17" s="12"/>
-      <c r="E17" s="10"/>
-      <c r="F17" s="37"/>
-      <c r="G17" s="37"/>
-      <c r="H17" s="37"/>
-      <c r="I17" s="37"/>
-      <c r="J17" s="37"/>
-      <c r="K17" s="37"/>
-      <c r="L17" s="10"/>
-      <c r="M17" s="10"/>
-      <c r="N17" s="10"/>
-      <c r="O17" s="10"/>
-      <c r="P17" s="10"/>
-      <c r="Q17" s="10"/>
+      <c r="B17" s="27"/>
+      <c r="C17" s="27"/>
+      <c r="D17" s="28"/>
+      <c r="E17" s="27"/>
+      <c r="F17" s="30"/>
+      <c r="G17" s="30"/>
+      <c r="H17" s="30"/>
+      <c r="I17" s="30"/>
+      <c r="J17" s="30"/>
+      <c r="K17" s="30"/>
+      <c r="L17" s="27"/>
+      <c r="M17" s="27"/>
+      <c r="N17" s="27"/>
+      <c r="O17" s="27"/>
+      <c r="P17" s="27"/>
+      <c r="Q17" s="27"/>
       <c r="R17" s="8"/>
-      <c r="S17" s="10"/>
-      <c r="T17" s="10"/>
-      <c r="U17" s="10"/>
-      <c r="V17" s="10"/>
-      <c r="W17" s="10"/>
-      <c r="X17" s="13"/>
-      <c r="Y17" s="13"/>
-      <c r="Z17" s="13"/>
-      <c r="AA17" s="13"/>
-      <c r="AB17" s="13"/>
-      <c r="AC17" s="13"/>
-      <c r="AD17" s="10"/>
-      <c r="AE17" s="10"/>
-      <c r="AF17" s="10"/>
-      <c r="AG17" s="10"/>
-      <c r="AH17" s="10"/>
-      <c r="AI17" s="10"/>
+      <c r="S17" s="27"/>
+      <c r="T17" s="27"/>
+      <c r="U17" s="27"/>
+      <c r="V17" s="27"/>
+      <c r="W17" s="27"/>
+      <c r="X17" s="29"/>
+      <c r="Y17" s="29"/>
+      <c r="Z17" s="29"/>
+      <c r="AA17" s="29"/>
+      <c r="AB17" s="29"/>
+      <c r="AC17" s="29"/>
+      <c r="AD17" s="27"/>
+      <c r="AE17" s="27"/>
+      <c r="AF17" s="27"/>
+      <c r="AG17" s="27"/>
+      <c r="AH17" s="27"/>
+      <c r="AI17" s="27"/>
     </row>
     <row r="18" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="3"/>
-      <c r="B18" s="10"/>
-      <c r="C18" s="10"/>
-      <c r="D18" s="10"/>
-      <c r="E18" s="10"/>
-      <c r="F18" s="11" t="s">
+      <c r="B18" s="27"/>
+      <c r="C18" s="27"/>
+      <c r="D18" s="27"/>
+      <c r="E18" s="27"/>
+      <c r="F18" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="G18" s="11"/>
-      <c r="H18" s="11"/>
-      <c r="I18" s="11"/>
-      <c r="J18" s="11"/>
-      <c r="K18" s="11"/>
-      <c r="L18" s="10"/>
-      <c r="M18" s="10"/>
-      <c r="N18" s="10"/>
-      <c r="O18" s="10"/>
-      <c r="P18" s="10"/>
-      <c r="Q18" s="10"/>
+      <c r="G18" s="14"/>
+      <c r="H18" s="14"/>
+      <c r="I18" s="14"/>
+      <c r="J18" s="14"/>
+      <c r="K18" s="14"/>
+      <c r="L18" s="27"/>
+      <c r="M18" s="27"/>
+      <c r="N18" s="27"/>
+      <c r="O18" s="27"/>
+      <c r="P18" s="27"/>
+      <c r="Q18" s="27"/>
       <c r="R18" s="3"/>
-      <c r="S18" s="10"/>
-      <c r="T18" s="10"/>
-      <c r="U18" s="10"/>
-      <c r="V18" s="10"/>
-      <c r="W18" s="10"/>
-      <c r="X18" s="11" t="s">
+      <c r="S18" s="27"/>
+      <c r="T18" s="27"/>
+      <c r="U18" s="27"/>
+      <c r="V18" s="27"/>
+      <c r="W18" s="27"/>
+      <c r="X18" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="Y18" s="11"/>
-      <c r="Z18" s="11"/>
-      <c r="AA18" s="11"/>
-      <c r="AB18" s="11"/>
-      <c r="AC18" s="11"/>
-      <c r="AD18" s="10"/>
-      <c r="AE18" s="10"/>
-      <c r="AF18" s="10"/>
-      <c r="AG18" s="10"/>
-      <c r="AH18" s="10"/>
-      <c r="AI18" s="10"/>
+      <c r="Y18" s="14"/>
+      <c r="Z18" s="14"/>
+      <c r="AA18" s="14"/>
+      <c r="AB18" s="14"/>
+      <c r="AC18" s="14"/>
+      <c r="AD18" s="27"/>
+      <c r="AE18" s="27"/>
+      <c r="AF18" s="27"/>
+      <c r="AG18" s="27"/>
+      <c r="AH18" s="27"/>
+      <c r="AI18" s="27"/>
     </row>
   </sheetData>
   <mergeCells count="97">
-    <mergeCell ref="AC4:AF4"/>
-    <mergeCell ref="AC5:AF5"/>
-    <mergeCell ref="AC6:AF6"/>
-    <mergeCell ref="A5:H5"/>
-    <mergeCell ref="O5:T5"/>
-    <mergeCell ref="O4:T4"/>
-    <mergeCell ref="K4:N4"/>
-    <mergeCell ref="K5:N5"/>
-    <mergeCell ref="Z4:AB4"/>
-    <mergeCell ref="Z5:AB5"/>
-    <mergeCell ref="A6:H6"/>
-    <mergeCell ref="K6:N6"/>
-    <mergeCell ref="Z6:AB6"/>
-    <mergeCell ref="A11:C11"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="F11:G11"/>
-    <mergeCell ref="H11:I11"/>
-    <mergeCell ref="J11:K11"/>
+    <mergeCell ref="H1:Y1"/>
+    <mergeCell ref="U18:W18"/>
+    <mergeCell ref="X18:AC18"/>
+    <mergeCell ref="AD18:AE18"/>
+    <mergeCell ref="AF18:AG18"/>
+    <mergeCell ref="P18:Q18"/>
+    <mergeCell ref="S18:T18"/>
+    <mergeCell ref="P17:Q17"/>
+    <mergeCell ref="S17:T17"/>
+    <mergeCell ref="P16:Q16"/>
+    <mergeCell ref="P13:Q15"/>
+    <mergeCell ref="AD16:AE16"/>
+    <mergeCell ref="AF16:AG16"/>
+    <mergeCell ref="AB11:AC11"/>
+    <mergeCell ref="AB8:AC10"/>
+    <mergeCell ref="Z10:AA10"/>
+    <mergeCell ref="AH18:AI18"/>
+    <mergeCell ref="U10:W10"/>
+    <mergeCell ref="X10:Y10"/>
+    <mergeCell ref="AD17:AE17"/>
+    <mergeCell ref="AF17:AG17"/>
+    <mergeCell ref="AH17:AI17"/>
+    <mergeCell ref="U17:W17"/>
+    <mergeCell ref="X17:AC17"/>
+    <mergeCell ref="R16:AC16"/>
+    <mergeCell ref="A12:AI12"/>
+    <mergeCell ref="A13:A15"/>
+    <mergeCell ref="B13:C15"/>
+    <mergeCell ref="D13:E15"/>
+    <mergeCell ref="F13:K15"/>
+    <mergeCell ref="L13:M15"/>
+    <mergeCell ref="N13:O15"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="F18:K18"/>
+    <mergeCell ref="L18:M18"/>
+    <mergeCell ref="N18:O18"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="F17:K17"/>
+    <mergeCell ref="L17:M17"/>
+    <mergeCell ref="N17:O17"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="F16:K16"/>
+    <mergeCell ref="L16:M16"/>
+    <mergeCell ref="N16:O16"/>
+    <mergeCell ref="X11:Y11"/>
+    <mergeCell ref="U11:W11"/>
+    <mergeCell ref="AH16:AI16"/>
+    <mergeCell ref="AH13:AI15"/>
+    <mergeCell ref="X13:AC15"/>
+    <mergeCell ref="AD13:AE15"/>
+    <mergeCell ref="AF13:AG15"/>
+    <mergeCell ref="R13:R15"/>
+    <mergeCell ref="S13:T15"/>
+    <mergeCell ref="U13:W15"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="O6:T6"/>
+    <mergeCell ref="L11:M11"/>
+    <mergeCell ref="N11:O11"/>
+    <mergeCell ref="P11:Q11"/>
+    <mergeCell ref="R11:T11"/>
     <mergeCell ref="AD11:AG11"/>
     <mergeCell ref="AH11:AI11"/>
     <mergeCell ref="A8:AA9"/>
@@ -1584,69 +1631,24 @@
     <mergeCell ref="R10:T10"/>
     <mergeCell ref="AD8:AG10"/>
     <mergeCell ref="A10:C10"/>
-    <mergeCell ref="R13:R15"/>
-    <mergeCell ref="S13:T15"/>
-    <mergeCell ref="U13:W15"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="O6:T6"/>
-    <mergeCell ref="L11:M11"/>
-    <mergeCell ref="N11:O11"/>
-    <mergeCell ref="P11:Q11"/>
-    <mergeCell ref="R11:T11"/>
-    <mergeCell ref="X11:Y11"/>
-    <mergeCell ref="U11:W11"/>
-    <mergeCell ref="AH16:AI16"/>
-    <mergeCell ref="AH13:AI15"/>
-    <mergeCell ref="X13:AC15"/>
-    <mergeCell ref="AD13:AE15"/>
-    <mergeCell ref="AF13:AG15"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="F16:K16"/>
-    <mergeCell ref="L16:M16"/>
-    <mergeCell ref="N16:O16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="F17:K17"/>
-    <mergeCell ref="L17:M17"/>
-    <mergeCell ref="N17:O17"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="F18:K18"/>
-    <mergeCell ref="L18:M18"/>
-    <mergeCell ref="N18:O18"/>
-    <mergeCell ref="AH18:AI18"/>
-    <mergeCell ref="U10:W10"/>
-    <mergeCell ref="X10:Y10"/>
-    <mergeCell ref="AD17:AE17"/>
-    <mergeCell ref="AF17:AG17"/>
-    <mergeCell ref="AH17:AI17"/>
-    <mergeCell ref="U17:W17"/>
-    <mergeCell ref="X17:AC17"/>
-    <mergeCell ref="R16:AC16"/>
-    <mergeCell ref="A12:AI12"/>
-    <mergeCell ref="A13:A15"/>
-    <mergeCell ref="B13:C15"/>
-    <mergeCell ref="D13:E15"/>
-    <mergeCell ref="F13:K15"/>
-    <mergeCell ref="L13:M15"/>
-    <mergeCell ref="N13:O15"/>
-    <mergeCell ref="H1:Y1"/>
-    <mergeCell ref="U18:W18"/>
-    <mergeCell ref="X18:AC18"/>
-    <mergeCell ref="AD18:AE18"/>
-    <mergeCell ref="AF18:AG18"/>
-    <mergeCell ref="P18:Q18"/>
-    <mergeCell ref="S18:T18"/>
-    <mergeCell ref="P17:Q17"/>
-    <mergeCell ref="S17:T17"/>
-    <mergeCell ref="P16:Q16"/>
-    <mergeCell ref="P13:Q15"/>
-    <mergeCell ref="AD16:AE16"/>
-    <mergeCell ref="AF16:AG16"/>
-    <mergeCell ref="AB11:AC11"/>
-    <mergeCell ref="AB8:AC10"/>
-    <mergeCell ref="Z10:AA10"/>
+    <mergeCell ref="A11:C11"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="H11:I11"/>
+    <mergeCell ref="J11:K11"/>
+    <mergeCell ref="AC4:AF4"/>
+    <mergeCell ref="AC5:AF5"/>
+    <mergeCell ref="AC6:AF6"/>
+    <mergeCell ref="A5:H5"/>
+    <mergeCell ref="O5:T5"/>
+    <mergeCell ref="O4:T4"/>
+    <mergeCell ref="K4:N4"/>
+    <mergeCell ref="K5:N5"/>
+    <mergeCell ref="Z4:AB4"/>
+    <mergeCell ref="Z5:AB5"/>
+    <mergeCell ref="A6:H6"/>
+    <mergeCell ref="K6:N6"/>
+    <mergeCell ref="Z6:AB6"/>
   </mergeCells>
   <pageMargins left="0.22159090909090901" right="0.2" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="65" orientation="landscape" r:id="rId1"/>

</xml_diff>